<commit_message>
JAVA101 Adding Roadmap timeline and adding more details to first stages
</commit_message>
<xml_diff>
--- a/JAVA101.xlsx
+++ b/JAVA101.xlsx
@@ -12,23 +12,24 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" tabRatio="763"/>
   </bookViews>
   <sheets>
-    <sheet name="0Soporte" sheetId="1" r:id="rId1"/>
-    <sheet name="1Intro" sheetId="2" r:id="rId2"/>
-    <sheet name="2Design Patterns" sheetId="3" r:id="rId3"/>
-    <sheet name="3Generics&amp;Collections" sheetId="4" r:id="rId4"/>
-    <sheet name="4Testing&amp;Logging" sheetId="15" r:id="rId5"/>
-    <sheet name="5Functional Programming" sheetId="5" r:id="rId6"/>
-    <sheet name="6Concurrency&amp;NIO" sheetId="6" r:id="rId7"/>
-    <sheet name="7JDBC&amp;ORM" sheetId="7" r:id="rId8"/>
-    <sheet name="8RESTfulWebServices" sheetId="12" r:id="rId9"/>
-    <sheet name="9JavaFrameworks" sheetId="8" r:id="rId10"/>
-    <sheet name="10FrontEnd&amp;Ajax" sheetId="9" r:id="rId11"/>
-    <sheet name="NiceToHave_DevMethodologies" sheetId="16" r:id="rId12"/>
-    <sheet name="NiceToHave_BestPractices" sheetId="11" r:id="rId13"/>
-    <sheet name="NiceToHave_NoSQLDB" sheetId="13" r:id="rId14"/>
-    <sheet name="NiceToHave_uServices" sheetId="10" r:id="rId15"/>
-    <sheet name="NiceToHave_Solr" sheetId="14" r:id="rId16"/>
-    <sheet name="NiceToHave_CI" sheetId="18" r:id="rId17"/>
+    <sheet name="Roadmap" sheetId="19" r:id="rId1"/>
+    <sheet name="0Soporte" sheetId="1" r:id="rId2"/>
+    <sheet name="1Intro" sheetId="2" r:id="rId3"/>
+    <sheet name="2Design Patterns" sheetId="3" r:id="rId4"/>
+    <sheet name="3Generics&amp;Collections" sheetId="4" r:id="rId5"/>
+    <sheet name="4Testing&amp;Logging" sheetId="15" r:id="rId6"/>
+    <sheet name="5Functional Programming" sheetId="5" r:id="rId7"/>
+    <sheet name="6Concurrency&amp;NIO" sheetId="6" r:id="rId8"/>
+    <sheet name="7JDBC&amp;ORM" sheetId="7" r:id="rId9"/>
+    <sheet name="8RESTfulWebServices" sheetId="12" r:id="rId10"/>
+    <sheet name="9JavaFrameworks" sheetId="8" r:id="rId11"/>
+    <sheet name="10FrontEnd&amp;Ajax" sheetId="9" r:id="rId12"/>
+    <sheet name="NiceToHave_DevMethodologies" sheetId="16" r:id="rId13"/>
+    <sheet name="NiceToHave_BestPractices" sheetId="11" r:id="rId14"/>
+    <sheet name="NiceToHave_NoSQLDB" sheetId="13" r:id="rId15"/>
+    <sheet name="NiceToHave_uServices" sheetId="10" r:id="rId16"/>
+    <sheet name="NiceToHave_Solr" sheetId="14" r:id="rId17"/>
+    <sheet name="NiceToHave_CI" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="171">
   <si>
     <t>Java Building Blocks</t>
   </si>
@@ -268,15 +269,322 @@
   </si>
   <si>
     <t>Runtime, Checked, Errors</t>
+  </si>
+  <si>
+    <t>Interfase</t>
+  </si>
+  <si>
+    <t>Functional Interfase</t>
+  </si>
+  <si>
+    <t>Polimorfysm</t>
+  </si>
+  <si>
+    <t>Design Principles</t>
+  </si>
+  <si>
+    <t>Singleton</t>
+  </si>
+  <si>
+    <t>Builder</t>
+  </si>
+  <si>
+    <t>Inmutable Objects</t>
+  </si>
+  <si>
+    <t>Factory</t>
+  </si>
+  <si>
+    <t>https://maven.apache.org/guides/mini/guide-multiple-modules.html</t>
+  </si>
+  <si>
+    <t>modelo</t>
+  </si>
+  <si>
+    <t>persistencia</t>
+  </si>
+  <si>
+    <t>negocio</t>
+  </si>
+  <si>
+    <t>vista</t>
+  </si>
+  <si>
+    <t>webServices</t>
+  </si>
+  <si>
+    <t>core</t>
+  </si>
+  <si>
+    <t>MAVEN</t>
+  </si>
+  <si>
+    <t>Modulos</t>
+  </si>
+  <si>
+    <t>tipo:jar funcion: contener todo el modelo utilizado por la aplicación que puede ser utilizado para diferentes aplicaciones que busquen interactuar con ellos</t>
+  </si>
+  <si>
+    <t>tipo:jar funcion: contener al menos una implementacion para la persistencia del modelo</t>
+  </si>
+  <si>
+    <t>tipo:jar funcion: contener la logica de negocio requerida por la aplicación y dependiendo del tamaño o complejidad podran ser varios modulos</t>
+  </si>
+  <si>
+    <t>recursos-comunes</t>
+  </si>
+  <si>
+    <t>tipo:jar funcion: contener recursos estandares para utilizar en diferentes vistas como look and feel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tipo:war funcion modulo web que contendra una implementacion de UI </t>
+  </si>
+  <si>
+    <t>tipo:war funcion modulo web que publicara los web services a consumir por otras aplicaciones</t>
+  </si>
+  <si>
+    <t>tipo:jar funcion: incluir cualquier funcion generica desarrollada por la empresa(Ext StringUtils DateUtils ArrayUtils etc)</t>
+  </si>
+  <si>
+    <t>poc</t>
+  </si>
+  <si>
+    <t>tipo:jar funcion modulo para correr tutoriales</t>
+  </si>
+  <si>
+    <t>Independiente</t>
+  </si>
+  <si>
+    <t>SONAR</t>
+  </si>
+  <si>
+    <t>https://docs.sonarqube.org/display/SCAN/Analyzing+with+SonarQube+Scanner+for+Maven</t>
+  </si>
+  <si>
+    <t>SONAR+MAVEN</t>
+  </si>
+  <si>
+    <t>https://docs.sonarqube.org/display/SONAR/Get+Started+in+Two+Minutes</t>
+  </si>
+  <si>
+    <t>GITHUB</t>
+  </si>
+  <si>
+    <t>https://github.com/cisco2040/JAVA101</t>
+  </si>
+  <si>
+    <t>Training Material</t>
+  </si>
+  <si>
+    <t>https://www.tutorialspoint.com/object_oriented_analysis_design/ooad_object_oriented_design.htm</t>
+  </si>
+  <si>
+    <t>https://scotch.io/bar-talk/s-o-l-i-d-the-first-five-principles-of-object-oriented-design</t>
+  </si>
+  <si>
+    <t>Crearlos Para Cada CodeLine</t>
+  </si>
+  <si>
+    <t>parent-pom</t>
+  </si>
+  <si>
+    <t>tipo:pom</t>
+  </si>
+  <si>
+    <t>Workspace:</t>
+  </si>
+  <si>
+    <t>Within the POC project</t>
+  </si>
+  <si>
+    <t>Language Basics</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/javase/tutorial/java/nutsandbolts/index.html</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/javase/tutorial/java/javaOO/index.html</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/javase/tutorial/java/data/index.html</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/javase/tutorial/java/IandI/index.html</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/javase/tutorial/java/package/index.html</t>
+  </si>
+  <si>
+    <t>https://docs.oracle.com/javase/tutorial/essential/exceptions/</t>
+  </si>
+  <si>
+    <t>https://javapapers.com/core-java/fail-fast-vs-fail-safe/</t>
+  </si>
+  <si>
+    <t>https://tech.deepumohan.com/2013/01/when-to-use-interfaces-in-your.html</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Design Patterns</t>
+  </si>
+  <si>
+    <t>Generics &amp; Collections</t>
+  </si>
+  <si>
+    <t>Testing &amp; Logging</t>
+  </si>
+  <si>
+    <t>Functional Programming</t>
+  </si>
+  <si>
+    <t>Concurrency &amp; NIO</t>
+  </si>
+  <si>
+    <t>JDBC &amp; ORM</t>
+  </si>
+  <si>
+    <t>RESTful WebServices</t>
+  </si>
+  <si>
+    <t>Front End  &amp; Ajax</t>
+  </si>
+  <si>
+    <t>Development Methodologies</t>
+  </si>
+  <si>
+    <t>Best Practices</t>
+  </si>
+  <si>
+    <t>NoSQL DB</t>
+  </si>
+  <si>
+    <t>uServices</t>
+  </si>
+  <si>
+    <t>Solr</t>
+  </si>
+  <si>
+    <t>Continuous Integration</t>
+  </si>
+  <si>
+    <t>Vamos a revisar el conocimiento y herramientas no relacionadas con Java directamente pero que son necesarias para el seguimiento de los temas</t>
+  </si>
+  <si>
+    <t>Cubriremos un Repaso de OOP, Core API de Java, Diseño de Clases, Manejo de errores y excepciones</t>
+  </si>
+  <si>
+    <t>Cubriremos los patrones de diseño más comunes GOF, Singleton, MVC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cubriremos principalmente las diferentes implementaciones que tiene Java de collections </t>
+  </si>
+  <si>
+    <t>Para no desviarnos con SWING o con Aplicaciones Web o solo CLI se utilizaran los JUnits y Log4J para ejecutar los modulos o servicios que se creen hasta el momento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cambio de Paradigmas con Java 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Future y Non Blocking IO para trabajar con archivos </t>
+  </si>
+  <si>
+    <t>Cubriremos como ejecutar sentencias SQL de manera manual con JDBC y posteriormente usar Hibernate como ORM</t>
+  </si>
+  <si>
+    <t>Se basara en la utilización de JAX-RS para la implementación de un web service REST</t>
+  </si>
+  <si>
+    <t>Introduccion a Spring Core, Spring MVC, Spring Security y otros proyectos de Spring y Alternativas para investigar como Tapestry, Struts y App Servers</t>
+  </si>
+  <si>
+    <t>Front end Basico lo suficiente como para consumir y trabajar con web services</t>
+  </si>
+  <si>
+    <t>SCRUM, SAFe, TDD</t>
+  </si>
+  <si>
+    <t>Probablemente Casandra y MongoDB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search Engine </t>
+  </si>
+  <si>
+    <t>Jenkins y Sonar</t>
+  </si>
+  <si>
+    <t>Etapa</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Inicio Real</t>
+  </si>
+  <si>
+    <t>Fin Real</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Registrarse en Github</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Clonar Java101 Repo</t>
+  </si>
+  <si>
+    <t>Instalar Maven, Git, Eclipse STS, Sonar, Java8, Tomcat8, Oracle Express</t>
+  </si>
+  <si>
+    <t>Crear Esqueleto de artefactos para las 3 aplicaciones en el area designada de Java101 Repo</t>
+  </si>
+  <si>
+    <t>Pendiente:…</t>
+  </si>
+  <si>
+    <t>Tutorial de como agregar un junit y ejecutarlo con el ide</t>
+  </si>
+  <si>
+    <t>Crear una clase de Java y su prueba correspondiente para ejecutar el codigo desde el IDE</t>
+  </si>
+  <si>
+    <t>Java Frameworks Basico</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -315,14 +623,47 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -601,193 +942,456 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="8" t="str">
+        <f>"Duracion en dias:"&amp;SUM(D2:D32)&amp;" ó "&amp;(SUM(D2:D32)/5)&amp;" Semanas"</f>
+        <v>Duracion en dias:104 ó 20.8 Semanas</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="10">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="10">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="10">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>3</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D12" s="10">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>4</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="10">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>5</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="10">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>6</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="10">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>7</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D20" s="10">
+        <v>5</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>8</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D22" s="10">
+        <v>15</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>9</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" s="10">
+        <v>15</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>10</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D25" s="10">
+        <v>5</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D27" s="10">
+        <v>4</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="10">
+        <v>3</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D29" s="10">
+        <v>4</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="10">
+        <v>5</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D31" s="10">
+        <v>3</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D32" s="10">
+        <v>5</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="101.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -795,7 +1399,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -830,7 +1434,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -855,7 +1459,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -885,7 +1489,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -910,7 +1514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -933,31 +1537,6 @@
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
@@ -997,6 +1576,31 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1022,183 +1626,523 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A12" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" t="s">
-        <v>67</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" t="s">
-        <v>71</v>
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>91</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>6</v>
+      <c r="A23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>167</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B22" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1208,6 +2152,82 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="94" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -1232,7 +2252,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -1277,7 +2297,37 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -1302,32 +2352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -1355,34 +2380,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
JAVA101 updating excel for followup
</commit_message>
<xml_diff>
--- a/JAVA101.xlsx
+++ b/JAVA101.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="171">
   <si>
     <t>Java Building Blocks</t>
   </si>
@@ -532,28 +532,28 @@
     <t>-</t>
   </si>
   <si>
-    <t>Registrarse en Github</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Clonar Java101 Repo</t>
-  </si>
-  <si>
-    <t>Instalar Maven, Git, Eclipse STS, Sonar, Java8, Tomcat8, Oracle Express</t>
-  </si>
-  <si>
-    <t>Crear Esqueleto de artefactos para las 3 aplicaciones en el area designada de Java101 Repo</t>
-  </si>
-  <si>
     <t>Pendiente:…</t>
   </si>
   <si>
     <t>Tutorial de como agregar un junit y ejecutarlo con el ide</t>
   </si>
   <si>
-    <t>Crear una clase de Java y su prueba correspondiente para ejecutar el codigo desde el IDE</t>
-  </si>
-  <si>
     <t>Java Frameworks Basico</t>
+  </si>
+  <si>
+    <t>Estimado</t>
+  </si>
+  <si>
+    <t>Completado</t>
+  </si>
+  <si>
+    <t>Dias Restantes</t>
+  </si>
+  <si>
+    <t>Progreso</t>
+  </si>
+  <si>
+    <t>Total (Dias)</t>
   </si>
 </sst>
 </file>
@@ -627,7 +627,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -661,6 +661,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -942,38 +943,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="65.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="33.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
         <v>158</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="D1" s="8" t="str">
-        <f>"Duracion en dias:"&amp;SUM(D2:D32)&amp;" ó "&amp;(SUM(D2:D32)/5)&amp;" Semanas"</f>
-        <v>Duracion en dias:104 ó 20.8 Semanas</v>
+      <c r="D1" s="8" t="s">
+        <v>166</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -986,204 +1001,436 @@
       <c r="D2" s="10">
         <v>5</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="11"/>
+      <c r="E2" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>128</v>
+      </c>
       <c r="C3" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="11"/>
+        <v>144</v>
+      </c>
+      <c r="D3" s="10">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="13">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>129</v>
+      </c>
       <c r="C4" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="10">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="10">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="10">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="10">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="10">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" s="10">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D10" s="10">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>15</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="D8" s="10">
-        <v>5</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>2</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="D10" s="10">
-        <v>5</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C11" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11" s="10">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="10">
+        <v>5</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>5</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="10">
+        <v>4</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>4</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="10">
         <v>3</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="D12" s="10">
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
         <v>3</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D15" s="10">
         <v>4</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="D14" s="10">
-        <v>2</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>5</v>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>4</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>148</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="C16" s="12"/>
       <c r="D16" s="10">
-        <v>10</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D17" s="10">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="D18" s="10">
-        <v>10</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>5</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" s="10">
+        <v>104</v>
+      </c>
+      <c r="E19" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="F19" s="1">
+        <v>99.8</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="13">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>7</v>
       </c>
@@ -1198,16 +1445,22 @@
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="11"/>
       <c r="C21" s="12"/>
       <c r="D21" s="10"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>8</v>
       </c>
@@ -1222,21 +1475,27 @@
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
       <c r="D23" s="10"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>9</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>152</v>
@@ -1246,8 +1505,11 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>10</v>
       </c>
@@ -1262,16 +1524,22 @@
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="11"/>
       <c r="C26" s="12"/>
       <c r="D26" s="10"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>162</v>
       </c>
@@ -1286,8 +1554,11 @@
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>162</v>
       </c>
@@ -1300,8 +1571,11 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>162</v>
       </c>
@@ -1316,8 +1590,11 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>162</v>
       </c>
@@ -1330,8 +1607,11 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>162</v>
       </c>
@@ -1346,8 +1626,11 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>162</v>
       </c>
@@ -1362,6 +1645,9 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1941,10 +2227,10 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding updates to report and placeholder for project
</commit_message>
<xml_diff>
--- a/JAVA101.xlsx
+++ b/JAVA101.xlsx
@@ -13,23 +13,24 @@
   </bookViews>
   <sheets>
     <sheet name="Roadmap" sheetId="19" r:id="rId1"/>
-    <sheet name="0Soporte" sheetId="1" r:id="rId2"/>
-    <sheet name="1Intro" sheetId="2" r:id="rId3"/>
-    <sheet name="2Design Patterns" sheetId="3" r:id="rId4"/>
-    <sheet name="3Generics&amp;Collections" sheetId="4" r:id="rId5"/>
-    <sheet name="4Testing&amp;Logging" sheetId="15" r:id="rId6"/>
-    <sheet name="5Functional Programming" sheetId="5" r:id="rId7"/>
-    <sheet name="6Concurrency&amp;NIO" sheetId="6" r:id="rId8"/>
-    <sheet name="7JDBC&amp;ORM" sheetId="7" r:id="rId9"/>
-    <sheet name="8RESTfulWebServices" sheetId="12" r:id="rId10"/>
-    <sheet name="9JavaFrameworks" sheetId="8" r:id="rId11"/>
-    <sheet name="10FrontEnd&amp;Ajax" sheetId="9" r:id="rId12"/>
-    <sheet name="NiceToHave_DevMethodologies" sheetId="16" r:id="rId13"/>
-    <sheet name="NiceToHave_BestPractices" sheetId="11" r:id="rId14"/>
-    <sheet name="NiceToHave_NoSQLDB" sheetId="13" r:id="rId15"/>
-    <sheet name="NiceToHave_uServices" sheetId="10" r:id="rId16"/>
-    <sheet name="NiceToHave_Solr" sheetId="14" r:id="rId17"/>
-    <sheet name="NiceToHave_CI" sheetId="18" r:id="rId18"/>
+    <sheet name="NOTAS URLs" sheetId="20" r:id="rId2"/>
+    <sheet name="0Soporte" sheetId="1" r:id="rId3"/>
+    <sheet name="1Intro" sheetId="2" r:id="rId4"/>
+    <sheet name="2Design Patterns" sheetId="3" r:id="rId5"/>
+    <sheet name="3Generics&amp;Collections" sheetId="4" r:id="rId6"/>
+    <sheet name="4Testing&amp;Logging" sheetId="15" r:id="rId7"/>
+    <sheet name="5Functional Programming" sheetId="5" r:id="rId8"/>
+    <sheet name="6Concurrency&amp;NIO" sheetId="6" r:id="rId9"/>
+    <sheet name="7JDBC&amp;ORM" sheetId="7" r:id="rId10"/>
+    <sheet name="8RESTfulWebServices" sheetId="12" r:id="rId11"/>
+    <sheet name="9JavaFrameworks" sheetId="8" r:id="rId12"/>
+    <sheet name="10FrontEnd&amp;Ajax" sheetId="9" r:id="rId13"/>
+    <sheet name="NiceToHave_DevMethodologies" sheetId="16" r:id="rId14"/>
+    <sheet name="NiceToHave_BestPractices" sheetId="11" r:id="rId15"/>
+    <sheet name="NiceToHave_NoSQLDB" sheetId="13" r:id="rId16"/>
+    <sheet name="NiceToHave_uServices" sheetId="10" r:id="rId17"/>
+    <sheet name="NiceToHave_Solr" sheetId="14" r:id="rId18"/>
+    <sheet name="NiceToHave_CI" sheetId="18" r:id="rId19"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="184">
   <si>
     <t>Java Building Blocks</t>
   </si>
@@ -572,13 +573,34 @@
   </si>
   <si>
     <t>com.softtek</t>
+  </si>
+  <si>
+    <t>SCRUM</t>
+  </si>
+  <si>
+    <t>Progreso para 1 semana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">libre lunes 19 </t>
+  </si>
+  <si>
+    <t>26 27 28 vacaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">staples proyecto </t>
+  </si>
+  <si>
+    <t>Dependencias Spring Maven</t>
+  </si>
+  <si>
+    <t>http://www.baeldung.com/spring-with-maven#maven</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,8 +630,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -622,8 +651,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -646,12 +680,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -687,8 +733,11 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -968,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -985,9 +1034,10 @@
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="7" t="s">
         <v>148</v>
       </c>
@@ -1013,7 +1063,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1037,8 +1087,11 @@
       <c r="I2" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J2" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1062,8 +1115,11 @@
       <c r="I3" s="13">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="J3" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1087,8 +1143,11 @@
       <c r="I4" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1112,8 +1171,12 @@
       <c r="I5" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J5" s="16"/>
+      <c r="K5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1137,8 +1200,11 @@
       <c r="I6" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1163,7 +1229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1187,8 +1253,11 @@
       <c r="I8" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1212,8 +1281,11 @@
       <c r="I9" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1238,7 +1310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1262,8 +1334,11 @@
       <c r="I11" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1288,7 +1363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>152</v>
       </c>
@@ -1313,7 +1388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>152</v>
       </c>
@@ -1336,7 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>152</v>
       </c>
@@ -1361,7 +1436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>152</v>
       </c>
@@ -1685,6 +1760,36 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1710,7 +1815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -1745,7 +1850,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -1770,12 +1875,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1785,6 +1890,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>177</v>
+      </c>
+    </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
@@ -1800,7 +1910,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -1825,7 +1935,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -1848,31 +1958,6 @@
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
@@ -1912,6 +1997,31 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1937,10 +2047,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,7 +2449,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -2510,7 +2645,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
@@ -2586,7 +2721,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -2611,7 +2746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -2656,7 +2791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -2686,7 +2821,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A15"/>
   <sheetViews>
@@ -2709,34 +2844,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>